<commit_message>
bioassay 3 pam stuff
</commit_message>
<xml_diff>
--- a/data/2023-07-06_bioassay_3.xlsx
+++ b/data/2023-07-06_bioassay_3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cathe\Dropbox\PC\Desktop\MS Thesis\MS_Thesis_2023-2024\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{831F49B4-AFE2-4739-BC9E-30D05B01FE8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B732C0FE-DE3D-484B-B582-24DDCB2650A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{5CCCB351-C044-4070-A66C-061B35931ADB}"/>
+    <workbookView xWindow="0" yWindow="336" windowWidth="11496" windowHeight="12024" firstSheet="4" activeTab="6" xr2:uid="{5CCCB351-C044-4070-A66C-061B35931ADB}"/>
   </bookViews>
   <sheets>
     <sheet name="Chl" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="NO2" sheetId="4" r:id="rId4"/>
     <sheet name="All Nutrients" sheetId="5" r:id="rId5"/>
     <sheet name="All Nutrients zeroes" sheetId="6" r:id="rId6"/>
+    <sheet name="PAM" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -714,8 +715,30 @@
 </comments>
 </file>
 
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{24B88259-7E17-423E-B827-764EAA9C0848}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Total Chl a + Chl a isomers</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="74">
   <si>
     <t>Number</t>
   </si>
@@ -935,6 +958,9 @@
   <si>
     <t>NO3_5</t>
   </si>
+  <si>
+    <t>FvFm</t>
+  </si>
 </sst>
 </file>
 
@@ -1035,7 +1061,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1058,7 +1084,6 @@
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1376,7 +1401,7 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -6490,7 +6515,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D503721-5177-475D-B124-D41F3E74F654}">
   <dimension ref="A1:S56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B29"/>
     </sheetView>
   </sheetViews>
@@ -6739,11 +6764,11 @@
       <c r="B6" s="12">
         <v>45113</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="7">
         <v>0</v>
       </c>
       <c r="D6" s="7"/>
-      <c r="F6" s="14">
+      <c r="F6" s="7">
         <v>0</v>
       </c>
       <c r="G6" s="7"/>
@@ -6787,11 +6812,11 @@
       <c r="B7" s="12">
         <v>45113</v>
       </c>
-      <c r="C7" s="14">
+      <c r="C7" s="7">
         <v>0</v>
       </c>
       <c r="D7" s="7"/>
-      <c r="F7" s="14">
+      <c r="F7" s="7">
         <v>0</v>
       </c>
       <c r="G7" s="7"/>
@@ -6835,7 +6860,7 @@
       <c r="B8" s="12">
         <v>45113</v>
       </c>
-      <c r="C8" s="14">
+      <c r="C8" s="7">
         <v>0</v>
       </c>
       <c r="D8" s="7"/>
@@ -6883,7 +6908,7 @@
       <c r="B9" s="12">
         <v>45113</v>
       </c>
-      <c r="C9" s="14">
+      <c r="C9" s="7">
         <v>0</v>
       </c>
       <c r="D9" s="7"/>
@@ -7964,6 +7989,660 @@
     </row>
     <row r="56" spans="4:4">
       <c r="D56" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81674220-8498-41C1-B8D9-7D721B9C6F39}">
+  <dimension ref="A1:F36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6">
+        <v>45111</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6">
+        <v>45111</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="5"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6">
+        <v>45111</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="5"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6">
+        <v>45111</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="5"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6">
+        <v>45111</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6">
+        <v>45113</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="5"/>
+      <c r="F7">
+        <v>0.58399999999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="5">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6">
+        <v>45113</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8">
+        <v>0.57899999999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="5">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6">
+        <v>45113</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="F9">
+        <v>0.31900000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="5">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6">
+        <v>45113</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="5"/>
+      <c r="F10">
+        <v>0.55500000000000005</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="5">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6">
+        <v>45113</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="5"/>
+      <c r="F11">
+        <v>0.32800000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="5">
+        <v>11</v>
+      </c>
+      <c r="B12" s="6">
+        <v>45113</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="5"/>
+      <c r="F12">
+        <v>0.64400000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="5">
+        <v>12</v>
+      </c>
+      <c r="B13" s="6">
+        <v>45113</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="5"/>
+      <c r="F13">
+        <v>0.56100000000000005</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="5">
+        <v>13</v>
+      </c>
+      <c r="B14" s="6">
+        <v>45113</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="5"/>
+      <c r="F14">
+        <v>0.57799999999999996</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="5">
+        <v>14</v>
+      </c>
+      <c r="B15" s="6">
+        <v>45113</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="5"/>
+      <c r="F15">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="5">
+        <v>15</v>
+      </c>
+      <c r="B16" s="6">
+        <v>45113</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="5"/>
+      <c r="F16">
+        <v>0.64300000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="5">
+        <v>16</v>
+      </c>
+      <c r="B17" s="6">
+        <v>45113</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="5"/>
+      <c r="F17">
+        <v>0.34599999999999997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="5">
+        <v>17</v>
+      </c>
+      <c r="B18" s="6">
+        <v>45113</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="5"/>
+      <c r="F18">
+        <v>0.33600000000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="5">
+        <v>18</v>
+      </c>
+      <c r="B19" s="6">
+        <v>45113</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="5"/>
+      <c r="F19">
+        <v>0.58799999999999997</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="5">
+        <v>19</v>
+      </c>
+      <c r="B20" s="6">
+        <v>45113</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="5"/>
+      <c r="F20">
+        <v>0.58299999999999996</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="5">
+        <v>20</v>
+      </c>
+      <c r="B21" s="6">
+        <v>45113</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="5"/>
+      <c r="F21">
+        <v>0.54700000000000004</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="5">
+        <v>21</v>
+      </c>
+      <c r="B22" s="6">
+        <v>45113</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="5"/>
+      <c r="F22">
+        <v>0.59799999999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="5">
+        <v>22</v>
+      </c>
+      <c r="B23" s="6">
+        <v>45113</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="5"/>
+      <c r="F23">
+        <v>0.32600000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="5">
+        <v>23</v>
+      </c>
+      <c r="B24" s="6">
+        <v>45113</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="5"/>
+      <c r="F24">
+        <v>0.27600000000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="5">
+        <v>24</v>
+      </c>
+      <c r="B25" s="6">
+        <v>45113</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="5"/>
+      <c r="F25">
+        <v>0.46100000000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="5">
+        <v>25</v>
+      </c>
+      <c r="B26" s="6">
+        <v>45113</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="5"/>
+      <c r="F26">
+        <v>0.38100000000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="5">
+        <v>26</v>
+      </c>
+      <c r="B27" s="6">
+        <v>45113</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" s="5"/>
+      <c r="F27">
+        <v>0.621</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="5">
+        <v>27</v>
+      </c>
+      <c r="B28" s="6">
+        <v>45113</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" s="5"/>
+      <c r="F28">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="5">
+        <v>28</v>
+      </c>
+      <c r="B29" s="6">
+        <v>45113</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" s="5"/>
+      <c r="F29">
+        <v>0.65900000000000003</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="5">
+        <v>29</v>
+      </c>
+      <c r="B30" s="6">
+        <v>45113</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" s="5"/>
+      <c r="F30">
+        <v>0.66100000000000003</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="5">
+        <v>30</v>
+      </c>
+      <c r="B31" s="6">
+        <v>45113</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" s="5"/>
+      <c r="F31">
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="5">
+        <v>31</v>
+      </c>
+      <c r="B32" s="6">
+        <v>45113</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" s="5"/>
+      <c r="F32">
+        <v>0.65400000000000003</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="5">
+        <v>32</v>
+      </c>
+      <c r="B33" s="6">
+        <v>45113</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" s="5"/>
+      <c r="F33">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="5">
+        <v>33</v>
+      </c>
+      <c r="B34" s="6">
+        <v>45113</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E34" s="5"/>
+      <c r="F34">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="5">
+        <v>34</v>
+      </c>
+      <c r="B35" s="6">
+        <v>45113</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35" s="5"/>
+      <c r="F35">
+        <v>0.63800000000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="5">
+        <v>35</v>
+      </c>
+      <c r="B36" s="6">
+        <v>45113</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E36" s="5"/>
+      <c r="F36">
+        <v>0.33600000000000002</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>